<commit_message>
date format and skip missing rows
</commit_message>
<xml_diff>
--- a/test/test-excel.xlsx
+++ b/test/test-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/licro/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shosi/.julia/dev/EMAVisitors/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FF687C-6F4A-8546-B616-48F689FEFE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96C7B8C-4DD9-3E4E-AA8D-E8C4AB474C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1360" windowWidth="38400" windowHeight="23500" xr2:uid="{C5261A2F-1F4C-D949-BB36-7C68F3B6256C}"/>
+    <workbookView xWindow="-32060" yWindow="11260" windowWidth="30240" windowHeight="18880" xr2:uid="{C5261A2F-1F4C-D949-BB36-7C68F3B6256C}"/>
   </bookViews>
   <sheets>
     <sheet name="talk-schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Speakers' name</t>
   </si>
@@ -70,9 +70,6 @@
     <t>R113</t>
   </si>
   <si>
-    <t>2:00 - 2:30 PM</t>
-  </si>
-  <si>
     <t>Host</t>
   </si>
   <si>
@@ -88,27 +85,9 @@
     <t>ETH, Zurich</t>
   </si>
   <si>
-    <t>3:00 - 4:00 PM</t>
-  </si>
-  <si>
-    <t>10:00 - 10:30 AM</t>
-  </si>
-  <si>
-    <t>R222</t>
-  </si>
-  <si>
     <t>Seminar</t>
   </si>
   <si>
-    <t>Date: 06/10/2025</t>
-  </si>
-  <si>
-    <t>Room: LY325-R116</t>
-  </si>
-  <si>
-    <t>Time: 5:00 - 5:15 AM</t>
-  </si>
-  <si>
     <t>Yannick Heiser</t>
   </si>
   <si>
@@ -124,15 +103,6 @@
     <t>Shobhit Singhal</t>
   </si>
   <si>
-    <t>2:00 - 3:00 PM</t>
-  </si>
-  <si>
-    <t>R600</t>
-  </si>
-  <si>
-    <t>Title: The best talk</t>
-  </si>
-  <si>
     <t>PhD Student</t>
   </si>
   <si>
@@ -196,28 +166,43 @@
     <t>Other members</t>
   </si>
   <si>
-    <t>R700</t>
-  </si>
-  <si>
-    <t>7:00 - 8:00 AM</t>
-  </si>
-  <si>
-    <t>Isabela Gomes</t>
-  </si>
-  <si>
-    <t>isabela@hotmail.com</t>
-  </si>
-  <si>
     <t>Accommodation</t>
   </si>
   <si>
-    <t>Name: 1 Hotel Copenhagen</t>
-  </si>
-  <si>
-    <t>Address: Krystalgade 22, 1172 Copenhagen, Denmark</t>
-  </si>
-  <si>
-    <t>Google Maps: https://maps.app.goo.gl/w4DDhpL6Kiy48AfHA</t>
+    <t>Ezzat Elokda</t>
+  </si>
+  <si>
+    <t>elokdae@ethz.ch</t>
+  </si>
+  <si>
+    <t>Address: Lundtoftegårdsvej 12, 2800 Kongens Lyngby</t>
+  </si>
+  <si>
+    <t>Name: Four Points Flex by Sheraton Lyngby</t>
+  </si>
+  <si>
+    <t>18/09/2025</t>
+  </si>
+  <si>
+    <t>13:00 - 14:00</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00</t>
+  </si>
+  <si>
+    <t>Room: LY325-R113</t>
+  </si>
+  <si>
+    <t>Time: 10:00 - 11:00</t>
+  </si>
+  <si>
+    <t>Date: 18/09/2025</t>
+  </si>
+  <si>
+    <t>Title: Aligning the "Socio" in Socio-Technical Control: Trustworthy, Fair, and Efficient Resource Allocation with Karma Economies</t>
+  </si>
+  <si>
+    <t>Google Maps: https://share.google/o8XML8eIcPmbasHbG</t>
   </si>
 </sst>
 </file>
@@ -625,7 +610,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,13 +638,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -677,50 +662,50 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E2" s="5">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
-        <v>45818</v>
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3">
-        <v>45818</v>
+        <v>49</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -730,49 +715,40 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="9" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="6">
-        <v>45818</v>
+        <v>48</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="6">
-        <v>45818</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="1"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -780,21 +756,13 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="6">
-        <v>45818</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="1"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -802,18 +770,10 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="6">
-        <v>45819</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -821,18 +781,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F7" s="5"/>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="6">
-        <v>45820</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -840,49 +792,25 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F8" s="5"/>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="6">
-        <v>45819</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F9" s="5"/>
-      <c r="G9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="6">
-        <v>45820</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F10" s="5"/>
-      <c r="G10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="6">
-        <v>45819</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G11" s="1"/>
@@ -927,13 +855,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -941,10 +869,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -952,87 +880,87 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1068,24 +996,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>